<commit_message>
OnGotHited trigger context test + Evade Status Effect
</commit_message>
<xml_diff>
--- a/documentation/StatusEffect Database.xlsx
+++ b/documentation/StatusEffect Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC0015E-531D-468A-850A-75A5223F6106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABAC0D7-78F5-4CE0-A813-0CD984E1291E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,9 +228,6 @@
     <t>Recover mp each turn</t>
   </si>
   <si>
-    <t>Make it easily to hit</t>
-  </si>
-  <si>
     <t>true(expire when the target got hited)</t>
   </si>
   <si>
@@ -337,6 +334,9 @@
   </si>
   <si>
     <t>minus 50% accuracy and remove Precision</t>
+  </si>
+  <si>
+    <t>Evade Status is removed. Can not get the Evade Status.</t>
   </si>
 </sst>
 </file>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +780,7 @@
         <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>45</v>
@@ -995,7 +995,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>45</v>
@@ -1063,30 +1063,30 @@
         <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>45</v>
@@ -1114,7 +1114,7 @@
         <v>34</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>49</v>
@@ -1137,7 +1137,7 @@
         <v>45</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
         <v>35</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>49</v>
@@ -1165,7 +1165,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>45</v>
@@ -1182,13 +1182,13 @@
         <v>36</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1199,13 +1199,13 @@
         <v>17</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1216,7 +1216,7 @@
         <v>37</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>49</v>
@@ -1250,7 +1250,7 @@
         <v>38</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>49</v>
@@ -1264,10 +1264,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>45</v>
@@ -1284,7 +1284,7 @@
         <v>39</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>49</v>
@@ -1301,7 +1301,7 @@
         <v>19</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>45</v>
@@ -1318,13 +1318,13 @@
         <v>40</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1335,13 +1335,13 @@
         <v>20</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1352,13 +1352,13 @@
         <v>41</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1369,7 +1369,7 @@
         <v>21</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>45</v>
@@ -1386,7 +1386,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>49</v>
@@ -1403,13 +1403,13 @@
         <v>22</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>43</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>49</v>
@@ -1437,7 +1437,7 @@
         <v>23</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>45</v>
@@ -1451,16 +1451,16 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Disable logic in the BattleManager + freeze Status Effect
</commit_message>
<xml_diff>
--- a/documentation/StatusEffect Database.xlsx
+++ b/documentation/StatusEffect Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7955932D-8748-4BE1-91D7-B53EEC39CCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D94908-4A83-4D16-8EA4-2C061CE33899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -719,7 +719,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,20 +851,20 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OnDamageDelt trigger context text + LifeSteal Status Effect
</commit_message>
<xml_diff>
--- a/documentation/StatusEffect Database.xlsx
+++ b/documentation/StatusEffect Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34BFBAE-C1BD-49F2-A6D1-EA3E8E396DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021054E4-FA1E-4DC9-9C37-A2A4D019EE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="103">
   <si>
     <t>StatusID</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Adrenaline</t>
   </si>
   <si>
-    <t>Fury</t>
-  </si>
-  <si>
     <t>Focus</t>
   </si>
   <si>
@@ -267,12 +264,6 @@
     <t>Can not escape battle</t>
   </si>
   <si>
-    <t>Buffs damage by 100%. Can only use damage skills</t>
-  </si>
-  <si>
-    <t>true(3-5)</t>
-  </si>
-  <si>
     <t>May change the target of the skills</t>
   </si>
   <si>
@@ -337,6 +328,12 @@
   </si>
   <si>
     <t>Can not get Disabled</t>
+  </si>
+  <si>
+    <t>LifeSteal</t>
+  </si>
+  <si>
+    <t>Heals when do damage.</t>
   </si>
 </sst>
 </file>
@@ -718,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +743,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -757,13 +754,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -774,13 +771,13 @@
         <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -791,13 +788,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -808,13 +805,13 @@
         <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -825,13 +822,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -842,13 +839,13 @@
         <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -859,13 +856,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -876,13 +873,13 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,13 +890,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -910,13 +907,13 @@
         <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -927,13 +924,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -944,13 +941,13 @@
         <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -961,13 +958,13 @@
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -978,13 +975,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -995,13 +992,13 @@
         <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1009,16 +1006,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,13 +1026,13 @@
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1046,13 +1043,13 @@
         <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1063,13 +1060,13 @@
         <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1080,13 +1077,13 @@
         <v>32</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1097,13 +1094,13 @@
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1114,13 +1111,13 @@
         <v>33</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1131,13 +1128,13 @@
         <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1148,13 +1145,13 @@
         <v>34</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1165,13 +1162,13 @@
         <v>16</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1182,13 +1179,13 @@
         <v>35</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1199,13 +1196,13 @@
         <v>17</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1216,13 +1213,13 @@
         <v>36</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1233,13 +1230,13 @@
         <v>18</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1250,13 +1247,13 @@
         <v>37</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1264,16 +1261,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1284,13 +1281,13 @@
         <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1301,30 +1298,30 @@
         <v>19</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>81</v>
+      <c r="B35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1335,13 +1332,13 @@
         <v>20</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1349,16 +1346,16 @@
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1369,13 +1366,13 @@
         <v>21</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1383,16 +1380,16 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1403,13 +1400,13 @@
         <v>22</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1417,16 +1414,16 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1437,13 +1434,13 @@
         <v>23</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1451,16 +1448,16 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Taunt status effect (Debbuf)
</commit_message>
<xml_diff>
--- a/documentation/StatusEffect Database.xlsx
+++ b/documentation/StatusEffect Database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E122F81-656D-4458-869E-E7A5D65B602C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243C5CA8-B440-4044-86D8-FF1467B50381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,20 +886,20 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>